<commit_message>
Optimierungskapitel des ARM angefangen
</commit_message>
<xml_diff>
--- a/Results/Results2.xlsx
+++ b/Results/Results2.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="20">
   <si>
     <t>MCL1</t>
   </si>
@@ -123,6 +123,283 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ARM!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extraction</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ARM!$B$14:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MCL1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MCL2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MCL3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MCL4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ARM!$B$15:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1439</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>481</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ARM!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Processing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ARM!$B$14:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MCL1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MCL2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MCL3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MCL4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ARM!$B$16:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>141.91999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ARM!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Classification</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>ARM!$B$14:$E$14</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>MCL1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>MCL2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MCL3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>MCL4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ARM!$B$17:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.4500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="49657728"/>
+        <c:axId val="51249152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="49657728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51249152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51249152"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Laufzeit in [ms]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="49657728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.70000000000000007" r="0.70000000000000007" t="0.78740157499999996" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC19" sqref="AC19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -846,7 +1123,7 @@
         <v>1726.26</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:AD7" si="0">SUM(C3:C5)</f>
+        <f t="shared" ref="C7:AC7" si="0">SUM(C3:C5)</f>
         <v>563.86</v>
       </c>
       <c r="D7">
@@ -952,6 +1229,83 @@
       <c r="AC7">
         <f t="shared" si="0"/>
         <v>94.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f>D3</f>
+        <v>531</v>
+      </c>
+      <c r="C15">
+        <f>K3</f>
+        <v>1439</v>
+      </c>
+      <c r="D15">
+        <f>R3</f>
+        <v>60</v>
+      </c>
+      <c r="E15">
+        <f>Y3</f>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:B17" si="1">D4</f>
+        <v>1.4</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:C17" si="2">K4</f>
+        <v>141.91999999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D17" si="3">R4</f>
+        <v>5.57</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ref="E16:E17" si="4">Y4</f>
+        <v>17.73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="2"/>
+        <v>7.72</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>6.02</v>
       </c>
     </row>
   </sheetData>
@@ -962,6 +1316,8 @@
     <mergeCell ref="W1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>